<commit_message>
new images and removed collective characters
</commit_message>
<xml_diff>
--- a/input/interchangeability.xlsx
+++ b/input/interchangeability.xlsx
@@ -724,7 +724,7 @@
         <v>68</v>
       </c>
       <c r="C2">
-        <v>0.6516277327779</v>
+        <v>384</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -738,7 +738,7 @@
         <v>69</v>
       </c>
       <c r="C3">
-        <v>0.610243452739576</v>
+        <v>160</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -752,7 +752,7 @@
         <v>24</v>
       </c>
       <c r="C4">
-        <v>0.285077053455079</v>
+        <v>32</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -766,7 +766,7 @@
         <v>78</v>
       </c>
       <c r="C5">
-        <v>0.703115955119589</v>
+        <v>347</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -780,7 +780,7 @@
         <v>78</v>
       </c>
       <c r="C6">
-        <v>0.703115955119589</v>
+        <v>347</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -794,7 +794,7 @@
         <v>40</v>
       </c>
       <c r="C7">
-        <v>0.466900346673698</v>
+        <v>85</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -808,7 +808,7 @@
         <v>27</v>
       </c>
       <c r="C8">
-        <v>0.348960003163594</v>
+        <v>49</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -822,7 +822,7 @@
         <v>52</v>
       </c>
       <c r="C9">
-        <v>0.556622670594364</v>
+        <v>195</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -836,7 +836,7 @@
         <v>21</v>
       </c>
       <c r="C10">
-        <v>0.287649915892631</v>
+        <v>33</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -850,7 +850,7 @@
         <v>45</v>
       </c>
       <c r="C11">
-        <v>0.470387696416274</v>
+        <v>102</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -864,7 +864,7 @@
         <v>125</v>
       </c>
       <c r="C12">
-        <v>0.956312298068269</v>
+        <v>715</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -878,7 +878,7 @@
         <v>34</v>
       </c>
       <c r="C13">
-        <v>0.360211776162798</v>
+        <v>57</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -892,7 +892,7 @@
         <v>31</v>
       </c>
       <c r="C14">
-        <v>0.258228902321574</v>
+        <v>58</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -906,7 +906,7 @@
         <v>129</v>
       </c>
       <c r="C15">
-        <v>0.955570203162686</v>
+        <v>506</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -920,7 +920,7 @@
         <v>129</v>
       </c>
       <c r="C16">
-        <v>0.955570203162686</v>
+        <v>506</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -934,7 +934,7 @@
         <v>90</v>
       </c>
       <c r="C17">
-        <v>0.755670973262931</v>
+        <v>317</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -948,7 +948,7 @@
         <v>85</v>
       </c>
       <c r="C18">
-        <v>0.737413058912301</v>
+        <v>285</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -962,7 +962,7 @@
         <v>23</v>
       </c>
       <c r="C19">
-        <v>0.267753408706171</v>
+        <v>34</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -976,7 +976,7 @@
         <v>27</v>
       </c>
       <c r="C20">
-        <v>0.348960003163594</v>
+        <v>43</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -990,7 +990,7 @@
         <v>46</v>
       </c>
       <c r="C21">
-        <v>0.348632041978378</v>
+        <v>103</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -1004,7 +1004,7 @@
         <v>31</v>
       </c>
       <c r="C22">
-        <v>0.354195837797307</v>
+        <v>46</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -1018,7 +1018,7 @@
         <v>48</v>
       </c>
       <c r="C23">
-        <v>0.508299727683347</v>
+        <v>100</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -1032,7 +1032,7 @@
         <v>33</v>
       </c>
       <c r="C24">
-        <v>0.399906267344918</v>
+        <v>53</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -1046,7 +1046,7 @@
         <v>33</v>
       </c>
       <c r="C25">
-        <v>0.386449075289631</v>
+        <v>47</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -1060,7 +1060,7 @@
         <v>59</v>
       </c>
       <c r="C26">
-        <v>0.491112380910912</v>
+        <v>116</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -1074,7 +1074,7 @@
         <v>36</v>
       </c>
       <c r="C27">
-        <v>0.392921194169564</v>
+        <v>65</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -1088,7 +1088,7 @@
         <v>18</v>
       </c>
       <c r="C28">
-        <v>0.226559572468671</v>
+        <v>33</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -1102,7 +1102,7 @@
         <v>18</v>
       </c>
       <c r="C29">
-        <v>0.226559572468671</v>
+        <v>26</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -1116,7 +1116,7 @@
         <v>23</v>
       </c>
       <c r="C30">
-        <v>0.271101090299244</v>
+        <v>44</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -1130,7 +1130,7 @@
         <v>23</v>
       </c>
       <c r="C31">
-        <v>0.271101090299245</v>
+        <v>44</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -1144,7 +1144,7 @@
         <v>31</v>
       </c>
       <c r="C32">
-        <v>0.258228902321574</v>
+        <v>58</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -1158,7 +1158,7 @@
         <v>37</v>
       </c>
       <c r="C33">
-        <v>0.443471705412956</v>
+        <v>67</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -1172,7 +1172,7 @@
         <v>17</v>
       </c>
       <c r="C34">
-        <v>0.229792798692011</v>
+        <v>20</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -1186,7 +1186,7 @@
         <v>22</v>
       </c>
       <c r="C35">
-        <v>0.279089146755977</v>
+        <v>49</v>
       </c>
       <c r="D35">
         <v>1</v>
@@ -1200,7 +1200,7 @@
         <v>22</v>
       </c>
       <c r="C36">
-        <v>0.279089146755977</v>
+        <v>44</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -1214,7 +1214,7 @@
         <v>24</v>
       </c>
       <c r="C37">
-        <v>0.319610377157926</v>
+        <v>25</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -1228,7 +1228,7 @@
         <v>23</v>
       </c>
       <c r="C38">
-        <v>0.19002018988731</v>
+        <v>27</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -1242,7 +1242,7 @@
         <v>60</v>
       </c>
       <c r="C39">
-        <v>0.585570238429704</v>
+        <v>160</v>
       </c>
       <c r="D39">
         <v>0</v>
@@ -1256,7 +1256,7 @@
         <v>104</v>
       </c>
       <c r="C40">
-        <v>0.850161435715377</v>
+        <v>465</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -1270,7 +1270,7 @@
         <v>104</v>
       </c>
       <c r="C41">
-        <v>0.847125931234578</v>
+        <v>441</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -1284,7 +1284,7 @@
         <v>24</v>
       </c>
       <c r="C42">
-        <v>0.220282457104605</v>
+        <v>29</v>
       </c>
       <c r="D42">
         <v>1</v>
@@ -1298,7 +1298,7 @@
         <v>129</v>
       </c>
       <c r="C43">
-        <v>0.955570203162685</v>
+        <v>501</v>
       </c>
       <c r="D43">
         <v>0</v>
@@ -1312,7 +1312,7 @@
         <v>129</v>
       </c>
       <c r="C44">
-        <v>0.955570203162685</v>
+        <v>501</v>
       </c>
       <c r="D44">
         <v>0</v>
@@ -1326,7 +1326,7 @@
         <v>33</v>
       </c>
       <c r="C45">
-        <v>0.367438086542138</v>
+        <v>51</v>
       </c>
       <c r="D45">
         <v>0</v>
@@ -1340,7 +1340,7 @@
         <v>23</v>
       </c>
       <c r="C46">
-        <v>0.19002018988731</v>
+        <v>26</v>
       </c>
       <c r="D46">
         <v>1</v>
@@ -1354,7 +1354,7 @@
         <v>40</v>
       </c>
       <c r="C47">
-        <v>0.359633264282293</v>
+        <v>56</v>
       </c>
       <c r="D47">
         <v>1</v>
@@ -1368,7 +1368,7 @@
         <v>20</v>
       </c>
       <c r="C48">
-        <v>0.180655196047536</v>
+        <v>30</v>
       </c>
       <c r="D48">
         <v>1</v>
@@ -1382,7 +1382,7 @@
         <v>91</v>
       </c>
       <c r="C49">
-        <v>0.773285466027757</v>
+        <v>345</v>
       </c>
       <c r="D49">
         <v>0</v>
@@ -1396,7 +1396,7 @@
         <v>91</v>
       </c>
       <c r="C50">
-        <v>0.773285466027757</v>
+        <v>345</v>
       </c>
       <c r="D50">
         <v>0</v>
@@ -1410,7 +1410,7 @@
         <v>23</v>
       </c>
       <c r="C51">
-        <v>0.267753408706171</v>
+        <v>34</v>
       </c>
       <c r="D51">
         <v>1</v>
@@ -1424,7 +1424,7 @@
         <v>87</v>
       </c>
       <c r="C52">
-        <v>0.738945633019343</v>
+        <v>250</v>
       </c>
       <c r="D52">
         <v>0</v>
@@ -1438,7 +1438,7 @@
         <v>23</v>
       </c>
       <c r="C53">
-        <v>0.271101090299245</v>
+        <v>35</v>
       </c>
       <c r="D53">
         <v>1</v>
@@ -1452,7 +1452,7 @@
         <v>25</v>
       </c>
       <c r="C54">
-        <v>0.308710098933486</v>
+        <v>45</v>
       </c>
       <c r="D54">
         <v>1</v>
@@ -1466,7 +1466,7 @@
         <v>36</v>
       </c>
       <c r="C55">
-        <v>0.432143512068286</v>
+        <v>82</v>
       </c>
       <c r="D55">
         <v>1</v>
@@ -1480,7 +1480,7 @@
         <v>20</v>
       </c>
       <c r="C56">
-        <v>0.180655196047536</v>
+        <v>26</v>
       </c>
       <c r="D56">
         <v>1</v>
@@ -1494,7 +1494,7 @@
         <v>99</v>
       </c>
       <c r="C57">
-        <v>0.810719634483972</v>
+        <v>336</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -1508,7 +1508,7 @@
         <v>99</v>
       </c>
       <c r="C58">
-        <v>0.810719634483972</v>
+        <v>336</v>
       </c>
       <c r="D58">
         <v>0</v>
@@ -1522,7 +1522,7 @@
         <v>77</v>
       </c>
       <c r="C59">
-        <v>0.684767319882798</v>
+        <v>264</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -1536,7 +1536,7 @@
         <v>24</v>
       </c>
       <c r="C60">
-        <v>0.220282457104605</v>
+        <v>30</v>
       </c>
       <c r="D60">
         <v>1</v>
@@ -1550,7 +1550,7 @@
         <v>120</v>
       </c>
       <c r="C61">
-        <v>0.928302902784687</v>
+        <v>719</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -1564,7 +1564,7 @@
         <v>23</v>
       </c>
       <c r="C62">
-        <v>0.267753408706171</v>
+        <v>31</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -1578,7 +1578,7 @@
         <v>24</v>
       </c>
       <c r="C63">
-        <v>0.220282457104605</v>
+        <v>30</v>
       </c>
       <c r="D63">
         <v>1</v>
@@ -1592,7 +1592,7 @@
         <v>23</v>
       </c>
       <c r="C64">
-        <v>0.19002018988731</v>
+        <v>40</v>
       </c>
       <c r="D64">
         <v>1</v>
@@ -1606,7 +1606,7 @@
         <v>31</v>
       </c>
       <c r="C65">
-        <v>0.258228902321574</v>
+        <v>59</v>
       </c>
       <c r="D65">
         <v>1</v>
@@ -1620,7 +1620,7 @@
         <v>23</v>
       </c>
       <c r="C66">
-        <v>0.19002018988731</v>
+        <v>29</v>
       </c>
       <c r="D66">
         <v>1</v>
@@ -1634,7 +1634,7 @@
         <v>30</v>
       </c>
       <c r="C67">
-        <v>0.346578872661103</v>
+        <v>49</v>
       </c>
       <c r="D67">
         <v>1</v>
@@ -1648,7 +1648,7 @@
         <v>23</v>
       </c>
       <c r="C68">
-        <v>0.267753408706171</v>
+        <v>34</v>
       </c>
       <c r="D68">
         <v>1</v>
@@ -1662,7 +1662,7 @@
         <v>22</v>
       </c>
       <c r="C69">
-        <v>0.287300991425652</v>
+        <v>31</v>
       </c>
       <c r="D69">
         <v>1</v>
@@ -1676,7 +1676,7 @@
         <v>24</v>
       </c>
       <c r="C70">
-        <v>0.220282457104605</v>
+        <v>26</v>
       </c>
       <c r="D70">
         <v>1</v>
@@ -1690,7 +1690,7 @@
         <v>22</v>
       </c>
       <c r="C71">
-        <v>0.287300991425652</v>
+        <v>35</v>
       </c>
       <c r="D71">
         <v>1</v>
@@ -1704,7 +1704,7 @@
         <v>108</v>
       </c>
       <c r="C72">
-        <v>0.876415897247891</v>
+        <v>490</v>
       </c>
       <c r="D72">
         <v>0</v>
@@ -1718,7 +1718,7 @@
         <v>91</v>
       </c>
       <c r="C73">
-        <v>0.772703516115349</v>
+        <v>343</v>
       </c>
       <c r="D73">
         <v>0</v>
@@ -1732,7 +1732,7 @@
         <v>23</v>
       </c>
       <c r="C74">
-        <v>0.302315042951794</v>
+        <v>25</v>
       </c>
       <c r="D74">
         <v>1</v>
@@ -1746,7 +1746,7 @@
         <v>23</v>
       </c>
       <c r="C75">
-        <v>0.271101090299245</v>
+        <v>24</v>
       </c>
       <c r="D75">
         <v>0</v>
@@ -1760,7 +1760,7 @@
         <v>36</v>
       </c>
       <c r="C76">
-        <v>0.276791307317477</v>
+        <v>79</v>
       </c>
       <c r="D76">
         <v>1</v>
@@ -1774,7 +1774,7 @@
         <v>36</v>
       </c>
       <c r="C77">
-        <v>0.409734203010442</v>
+        <v>56</v>
       </c>
       <c r="D77">
         <v>0</v>
@@ -1788,7 +1788,7 @@
         <v>124</v>
       </c>
       <c r="C78">
-        <v>0.930443493581193</v>
+        <v>536</v>
       </c>
       <c r="D78">
         <v>0</v>
@@ -1802,7 +1802,7 @@
         <v>124</v>
       </c>
       <c r="C79">
-        <v>0.930443493581193</v>
+        <v>536</v>
       </c>
       <c r="D79">
         <v>0</v>
@@ -1816,7 +1816,7 @@
         <v>23</v>
       </c>
       <c r="C80">
-        <v>0.271101090299245</v>
+        <v>36</v>
       </c>
       <c r="D80">
         <v>1</v>
@@ -1830,7 +1830,7 @@
         <v>24</v>
       </c>
       <c r="C81">
-        <v>0.220282457104605</v>
+        <v>25</v>
       </c>
       <c r="D81">
         <v>0</v>
@@ -1844,7 +1844,7 @@
         <v>28</v>
       </c>
       <c r="C82">
-        <v>0.377306158107801</v>
+        <v>40</v>
       </c>
       <c r="D82">
         <v>1</v>
@@ -1858,7 +1858,7 @@
         <v>35</v>
       </c>
       <c r="C83">
-        <v>0.434851725768188</v>
+        <v>67</v>
       </c>
       <c r="D83">
         <v>1</v>
@@ -1872,7 +1872,7 @@
         <v>106</v>
       </c>
       <c r="C84">
-        <v>0.866418249584441</v>
+        <v>515</v>
       </c>
       <c r="D84">
         <v>0</v>
@@ -1886,7 +1886,7 @@
         <v>27</v>
       </c>
       <c r="C85">
-        <v>0.348960003163594</v>
+        <v>46</v>
       </c>
       <c r="D85">
         <v>0</v>
@@ -1900,7 +1900,7 @@
         <v>22</v>
       </c>
       <c r="C86">
-        <v>0.31448623040473</v>
+        <v>34</v>
       </c>
       <c r="D86">
         <v>0</v>
@@ -1914,7 +1914,7 @@
         <v>24</v>
       </c>
       <c r="C87">
-        <v>0.285077053455079</v>
+        <v>32</v>
       </c>
       <c r="D87">
         <v>1</v>
@@ -1928,7 +1928,7 @@
         <v>23</v>
       </c>
       <c r="C88">
-        <v>0.267753408706171</v>
+        <v>34</v>
       </c>
       <c r="D88">
         <v>1</v>
@@ -1942,7 +1942,7 @@
         <v>22</v>
       </c>
       <c r="C89">
-        <v>0.279089146755977</v>
+        <v>30</v>
       </c>
       <c r="D89">
         <v>1</v>
@@ -1956,7 +1956,7 @@
         <v>20</v>
       </c>
       <c r="C90">
-        <v>0.180655196047536</v>
+        <v>27</v>
       </c>
       <c r="D90">
         <v>1</v>
@@ -1970,7 +1970,7 @@
         <v>23</v>
       </c>
       <c r="C91">
-        <v>0.302315042951794</v>
+        <v>30</v>
       </c>
       <c r="D91">
         <v>1</v>
@@ -1984,7 +1984,7 @@
         <v>41</v>
       </c>
       <c r="C92">
-        <v>0.455367645292577</v>
+        <v>85</v>
       </c>
       <c r="D92">
         <v>1</v>
@@ -1998,7 +1998,7 @@
         <v>33</v>
       </c>
       <c r="C93">
-        <v>0.411581167499253</v>
+        <v>72</v>
       </c>
       <c r="D93">
         <v>1</v>
@@ -2012,7 +2012,7 @@
         <v>108</v>
       </c>
       <c r="C94">
-        <v>0.876415897247892</v>
+        <v>494</v>
       </c>
       <c r="D94">
         <v>0</v>
@@ -2026,7 +2026,7 @@
         <v>40</v>
       </c>
       <c r="C95">
-        <v>0.315746420016905</v>
+        <v>69</v>
       </c>
       <c r="D95">
         <v>0</v>
@@ -2040,7 +2040,7 @@
         <v>52</v>
       </c>
       <c r="C96">
-        <v>0.54928340026891</v>
+        <v>179</v>
       </c>
       <c r="D96">
         <v>0</v>
@@ -2054,7 +2054,7 @@
         <v>31</v>
       </c>
       <c r="C97">
-        <v>0.258228902321574</v>
+        <v>53</v>
       </c>
       <c r="D97">
         <v>1</v>
@@ -2068,7 +2068,7 @@
         <v>27</v>
       </c>
       <c r="C98">
-        <v>0.348960003163594</v>
+        <v>30</v>
       </c>
       <c r="D98">
         <v>1</v>
@@ -2082,7 +2082,7 @@
         <v>24</v>
       </c>
       <c r="C99">
-        <v>0.285077053455079</v>
+        <v>41</v>
       </c>
       <c r="D99">
         <v>1</v>
@@ -2096,7 +2096,7 @@
         <v>138</v>
       </c>
       <c r="C100">
-        <v>1</v>
+        <v>649</v>
       </c>
       <c r="D100">
         <v>0</v>
@@ -2110,7 +2110,7 @@
         <v>138</v>
       </c>
       <c r="C101">
-        <v>1</v>
+        <v>649</v>
       </c>
       <c r="D101">
         <v>0</v>
@@ -2124,7 +2124,7 @@
         <v>112</v>
       </c>
       <c r="C102">
-        <v>0.87078105241344</v>
+        <v>471</v>
       </c>
       <c r="D102">
         <v>0</v>
@@ -2138,7 +2138,7 @@
         <v>32</v>
       </c>
       <c r="C103">
-        <v>0.375155060159349</v>
+        <v>51</v>
       </c>
       <c r="D103">
         <v>0</v>
@@ -2152,7 +2152,7 @@
         <v>47</v>
       </c>
       <c r="C104">
-        <v>0.513785618972257</v>
+        <v>134</v>
       </c>
       <c r="D104">
         <v>0</v>
@@ -2166,7 +2166,7 @@
         <v>23</v>
       </c>
       <c r="C105">
-        <v>0.271101090299245</v>
+        <v>36</v>
       </c>
       <c r="D105">
         <v>1</v>
@@ -2180,7 +2180,7 @@
         <v>33</v>
       </c>
       <c r="C106">
-        <v>0.411581167499253</v>
+        <v>72</v>
       </c>
       <c r="D106">
         <v>1</v>
@@ -2194,7 +2194,7 @@
         <v>27</v>
       </c>
       <c r="C107">
-        <v>0.348960003163594</v>
+        <v>32</v>
       </c>
       <c r="D107">
         <v>0</v>
@@ -2208,7 +2208,7 @@
         <v>24</v>
       </c>
       <c r="C108">
-        <v>0.278079793490115</v>
+        <v>26</v>
       </c>
       <c r="D108">
         <v>1</v>
@@ -2222,7 +2222,7 @@
         <v>21</v>
       </c>
       <c r="C109">
-        <v>0.287649915892631</v>
+        <v>32</v>
       </c>
       <c r="D109">
         <v>1</v>
@@ -2236,7 +2236,7 @@
         <v>24</v>
       </c>
       <c r="C110">
-        <v>0.220282457104605</v>
+        <v>29</v>
       </c>
       <c r="D110">
         <v>1</v>
@@ -2250,7 +2250,7 @@
         <v>24</v>
       </c>
       <c r="C111">
-        <v>0.285077053455079</v>
+        <v>27</v>
       </c>
       <c r="D111">
         <v>1</v>
@@ -2264,7 +2264,7 @@
         <v>33</v>
       </c>
       <c r="C112">
-        <v>0.399906267344918</v>
+        <v>65</v>
       </c>
       <c r="D112">
         <v>0</v>
@@ -2278,7 +2278,7 @@
         <v>40</v>
       </c>
       <c r="C113">
-        <v>0.463957752934856</v>
+        <v>83</v>
       </c>
       <c r="D113">
         <v>0</v>
@@ -2292,7 +2292,7 @@
         <v>48</v>
       </c>
       <c r="C114">
-        <v>0.519862448445706</v>
+        <v>111</v>
       </c>
       <c r="D114">
         <v>0</v>
@@ -2306,7 +2306,7 @@
         <v>116</v>
       </c>
       <c r="C115">
-        <v>0.914203060752205</v>
+        <v>734</v>
       </c>
       <c r="D115">
         <v>0</v>
@@ -2320,7 +2320,7 @@
         <v>23</v>
       </c>
       <c r="C116">
-        <v>0.267753408706171</v>
+        <v>34</v>
       </c>
       <c r="D116">
         <v>0</v>
@@ -2334,7 +2334,7 @@
         <v>24</v>
       </c>
       <c r="C117">
-        <v>0.278079793490115</v>
+        <v>45</v>
       </c>
       <c r="D117">
         <v>1</v>
@@ -2348,7 +2348,7 @@
         <v>51</v>
       </c>
       <c r="C118">
-        <v>0.540776454935549</v>
+        <v>136</v>
       </c>
       <c r="D118">
         <v>0</v>
@@ -2362,7 +2362,7 @@
         <v>30</v>
       </c>
       <c r="C119">
-        <v>0.371829559609622</v>
+        <v>47</v>
       </c>
       <c r="D119">
         <v>0</v>
@@ -2376,7 +2376,7 @@
         <v>24</v>
       </c>
       <c r="C120">
-        <v>0.319610377157926</v>
+        <v>28</v>
       </c>
       <c r="D120">
         <v>0</v>
@@ -2390,7 +2390,7 @@
         <v>23</v>
       </c>
       <c r="C121">
-        <v>0.19002018988731</v>
+        <v>26</v>
       </c>
       <c r="D121">
         <v>1</v>

</xml_diff>